<commit_message>
rectified expected output customSheetsExampleUseCase.xlsx
</commit_message>
<xml_diff>
--- a/xmltoexcel/src/test/resources/expected-output/customSheetsExampleUseCase.xlsx
+++ b/xmltoexcel/src/test/resources/expected-output/customSheetsExampleUseCase.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>name</t>
   </si>
@@ -27,6 +27,9 @@
     <t>description_body</t>
   </si>
   <si>
+    <t>calories</t>
+  </si>
+  <si>
     <t>food1</t>
   </si>
   <si>
@@ -39,13 +42,13 @@
     <t>body1</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>food2</t>
   </si>
   <si>
     <t>$2</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>title</t>
@@ -108,52 +111,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
+      <c r="E1" t="s" s="0">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" t="s" s="0">
         <v>7</v>
       </c>
+      <c r="D2" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>9</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="A3" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
+      <c r="B3" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -170,35 +182,35 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>11</v>
+      <c r="B1" t="s" s="0">
+        <v>12</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
+      <c r="A2" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>7</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" t="s" s="0">
         <v>14</v>
       </c>
+      <c r="B3" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" t="s" s="0">
         <v>16</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>